<commit_message>
Project CRC Added to #15
</commit_message>
<xml_diff>
--- a/Structural Modeling/User CRC.xlsx
+++ b/Structural Modeling/User CRC.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1968" windowHeight="228" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1968" windowHeight="228"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
-    <sheet name="project" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>class name: user</t>
   </si>
@@ -99,9 +98,6 @@
     <t>tag</t>
   </si>
   <si>
-    <t>delete</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -225,12 +221,6 @@
     <t>relationships</t>
   </si>
   <si>
-    <t>class name: project</t>
-  </si>
-  <si>
-    <t>id : 2</t>
-  </si>
-  <si>
     <t>management_project_list</t>
   </si>
   <si>
@@ -247,15 +237,6 @@
   </si>
   <si>
     <t xml:space="preserve">association </t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
-    <t>view tasks</t>
-  </si>
-  <si>
-    <t>add/delete user to project</t>
   </si>
 </sst>
 </file>
@@ -583,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -728,20 +709,20 @@
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
@@ -749,7 +730,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>22</v>
@@ -757,7 +738,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -765,7 +746,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
@@ -773,47 +754,47 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -821,142 +802,142 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>21</v>
@@ -964,7 +945,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>22</v>
@@ -972,7 +953,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>23</v>
@@ -980,114 +961,22 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>